<commit_message>
end input much earlier, frame 27738
</commit_message>
<xml_diff>
--- a/RallyBike/FrameCompare.xlsx
+++ b/RallyBike/FrameCompare.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\RallyBike\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9FB6840-DB3A-4BC4-8E20-785DCFDEC9DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4976439-11D3-449D-874D-41C9FB0BB4F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44640" yWindow="1335" windowWidth="14490" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V6" sheetId="10" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="23">
   <si>
     <t>Place</t>
   </si>
@@ -108,12 +108,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]&quot;-&quot;[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -229,34 +236,35 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Accent1" xfId="5" builtinId="29"/>
@@ -577,11 +585,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E7E52CC-3356-4254-B5E7-E1B0B655F38D}">
-  <dimension ref="A1:F318"/>
+  <dimension ref="A1:F317"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -617,7 +625,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="3">
-        <f t="shared" ref="D2:D34" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
+        <f t="shared" ref="D2:D33" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
         <v>0</v>
       </c>
       <c r="F2" s="2"/>
@@ -1075,43 +1083,45 @@
     </row>
     <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B33" s="2">
-        <v>28710</v>
+        <v>29684</v>
       </c>
       <c r="C33" s="2">
-        <v>31003</v>
+        <v>30368</v>
       </c>
       <c r="D33" s="3">
         <f t="shared" si="0"/>
-        <v>2293</v>
-      </c>
-      <c r="E33" s="2">
-        <v>29677</v>
-      </c>
-      <c r="F33" t="s">
-        <v>22</v>
+        <v>684</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B34" s="2">
-        <v>29684</v>
+        <v>27738</v>
       </c>
       <c r="C34" s="2">
-        <v>30368</v>
+        <v>31003</v>
       </c>
       <c r="D34" s="3">
-        <f t="shared" si="0"/>
-        <v>684</v>
+        <f t="shared" ref="D34" si="1">IF(C34&lt;&gt;"",IF(B34&lt;&gt;"",C34-B34,"-"), "-")</f>
+        <v>3265</v>
+      </c>
+      <c r="E34" s="2">
+        <v>29677</v>
+      </c>
+      <c r="F34" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
-      <c r="B35" s="2"/>
+      <c r="B35" s="16" t="s">
+        <v>2</v>
+      </c>
       <c r="C35" s="2"/>
       <c r="D35" s="3"/>
     </row>
@@ -1122,13 +1132,13 @@
       <c r="D36" s="3"/>
     </row>
     <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
+      <c r="A37" s="10"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="10"/>
+      <c r="A38" s="8"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="3"/>
@@ -1182,16 +1192,16 @@
       <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="8"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="3"/>
+      <c r="A47" s="9"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="6"/>
     </row>
     <row r="48" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="9"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="6"/>
+      <c r="A48" s="8"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="3"/>
     </row>
     <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="8"/>
@@ -1206,16 +1216,16 @@
       <c r="D50" s="3"/>
     </row>
     <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="8"/>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="3"/>
+      <c r="A51" s="9"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="6"/>
     </row>
     <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A52" s="9"/>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="6"/>
+      <c r="A52" s="8"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="3"/>
     </row>
     <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="8"/>
@@ -1230,16 +1240,16 @@
       <c r="D54" s="3"/>
     </row>
     <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A55" s="8"/>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="3"/>
+      <c r="A55" s="9"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="6"/>
     </row>
     <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A56" s="9"/>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="6"/>
+      <c r="A56" s="8"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="3"/>
     </row>
     <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="8"/>
@@ -1278,16 +1288,16 @@
       <c r="D62" s="3"/>
     </row>
     <row r="63" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A63" s="8"/>
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
-      <c r="D63" s="3"/>
+      <c r="A63" s="9"/>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="6"/>
     </row>
     <row r="64" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A64" s="9"/>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="6"/>
+      <c r="A64" s="8"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="3"/>
     </row>
     <row r="65" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="8"/>
@@ -1326,16 +1336,16 @@
       <c r="D70" s="3"/>
     </row>
     <row r="71" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A71" s="8"/>
-      <c r="B71" s="2"/>
-      <c r="C71" s="2"/>
-      <c r="D71" s="3"/>
+      <c r="A71" s="9"/>
+      <c r="B71" s="5"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="6"/>
     </row>
     <row r="72" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A72" s="9"/>
-      <c r="B72" s="5"/>
-      <c r="C72" s="5"/>
-      <c r="D72" s="6"/>
+      <c r="A72" s="8"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="3"/>
     </row>
     <row r="73" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="8"/>
@@ -1374,20 +1384,20 @@
       <c r="D78" s="3"/>
     </row>
     <row r="79" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A79" s="8"/>
-      <c r="B79" s="2"/>
-      <c r="C79" s="2"/>
-      <c r="D79" s="3"/>
+      <c r="A79" s="9"/>
+      <c r="B79" s="5"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="6"/>
     </row>
     <row r="80" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A80" s="9"/>
-      <c r="B80" s="5"/>
-      <c r="C80" s="5"/>
-      <c r="D80" s="6"/>
+      <c r="A80" s="8"/>
+      <c r="B80" s="10"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="3"/>
     </row>
     <row r="81" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="8"/>
-      <c r="B81" s="10"/>
+      <c r="B81" s="2"/>
       <c r="C81" s="2"/>
       <c r="D81" s="3"/>
     </row>
@@ -1416,19 +1426,19 @@
       <c r="D85" s="3"/>
     </row>
     <row r="86" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A86" s="8"/>
-      <c r="B86" s="2"/>
-      <c r="C86" s="2"/>
-      <c r="D86" s="3"/>
+      <c r="A86" s="9"/>
+      <c r="B86" s="5"/>
+      <c r="C86" s="5"/>
+      <c r="D86" s="6"/>
     </row>
     <row r="87" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A87" s="9"/>
-      <c r="B87" s="5"/>
-      <c r="C87" s="5"/>
-      <c r="D87" s="6"/>
+      <c r="A87" s="8"/>
+      <c r="B87" s="2"/>
+      <c r="C87" s="2"/>
+      <c r="D87" s="3"/>
     </row>
     <row r="88" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A88" s="8"/>
+      <c r="A88" s="10"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
       <c r="D88" s="3"/>
@@ -1452,22 +1462,22 @@
       <c r="D91" s="3"/>
     </row>
     <row r="92" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A92" s="10"/>
+      <c r="A92" s="8"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
       <c r="D92" s="3"/>
     </row>
     <row r="93" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A93" s="8"/>
-      <c r="B93" s="2"/>
-      <c r="C93" s="2"/>
-      <c r="D93" s="3"/>
+      <c r="A93" s="9"/>
+      <c r="B93" s="5"/>
+      <c r="C93" s="5"/>
+      <c r="D93" s="6"/>
     </row>
     <row r="94" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A94" s="9"/>
-      <c r="B94" s="5"/>
-      <c r="C94" s="5"/>
-      <c r="D94" s="6"/>
+      <c r="A94" s="8"/>
+      <c r="B94" s="2"/>
+      <c r="C94" s="2"/>
+      <c r="D94" s="3"/>
     </row>
     <row r="95" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="8"/>
@@ -1506,16 +1516,16 @@
       <c r="D100" s="3"/>
     </row>
     <row r="101" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A101" s="8"/>
-      <c r="B101" s="2"/>
-      <c r="C101" s="2"/>
-      <c r="D101" s="3"/>
+      <c r="A101" s="9"/>
+      <c r="B101" s="5"/>
+      <c r="C101" s="5"/>
+      <c r="D101" s="6"/>
     </row>
     <row r="102" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A102" s="9"/>
-      <c r="B102" s="5"/>
-      <c r="C102" s="5"/>
-      <c r="D102" s="6"/>
+      <c r="A102" s="8"/>
+      <c r="B102" s="2"/>
+      <c r="C102" s="2"/>
+      <c r="D102" s="3"/>
     </row>
     <row r="103" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" s="8"/>
@@ -1530,13 +1540,13 @@
       <c r="D104" s="3"/>
     </row>
     <row r="105" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A105" s="8"/>
+      <c r="A105" s="10"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
       <c r="D105" s="3"/>
     </row>
     <row r="106" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A106" s="10"/>
+      <c r="A106" s="8"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
       <c r="D106" s="3"/>
@@ -1560,16 +1570,16 @@
       <c r="D109" s="3"/>
     </row>
     <row r="110" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A110" s="8"/>
-      <c r="B110" s="2"/>
-      <c r="C110" s="2"/>
-      <c r="D110" s="3"/>
+      <c r="A110" s="9"/>
+      <c r="B110" s="5"/>
+      <c r="C110" s="5"/>
+      <c r="D110" s="6"/>
     </row>
     <row r="111" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A111" s="9"/>
-      <c r="B111" s="5"/>
-      <c r="C111" s="5"/>
-      <c r="D111" s="6"/>
+      <c r="A111" s="8"/>
+      <c r="B111" s="2"/>
+      <c r="C111" s="2"/>
+      <c r="D111" s="3"/>
     </row>
     <row r="112" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A112" s="8"/>
@@ -1632,16 +1642,16 @@
       <c r="D121" s="3"/>
     </row>
     <row r="122" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A122" s="8"/>
-      <c r="B122" s="2"/>
-      <c r="C122" s="2"/>
-      <c r="D122" s="3"/>
+      <c r="A122" s="9"/>
+      <c r="B122" s="5"/>
+      <c r="C122" s="5"/>
+      <c r="D122" s="6"/>
     </row>
     <row r="123" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A123" s="9"/>
-      <c r="B123" s="5"/>
-      <c r="C123" s="5"/>
-      <c r="D123" s="6"/>
+      <c r="A123" s="8"/>
+      <c r="B123" s="2"/>
+      <c r="C123" s="2"/>
+      <c r="D123" s="3"/>
     </row>
     <row r="124" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A124" s="8"/>
@@ -1692,16 +1702,16 @@
       <c r="D131" s="3"/>
     </row>
     <row r="132" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A132" s="8"/>
-      <c r="B132" s="2"/>
-      <c r="C132" s="2"/>
-      <c r="D132" s="3"/>
+      <c r="A132" s="9"/>
+      <c r="B132" s="5"/>
+      <c r="C132" s="5"/>
+      <c r="D132" s="6"/>
     </row>
     <row r="133" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A133" s="9"/>
-      <c r="B133" s="5"/>
-      <c r="C133" s="5"/>
-      <c r="D133" s="6"/>
+      <c r="A133" s="8"/>
+      <c r="B133" s="2"/>
+      <c r="C133" s="2"/>
+      <c r="D133" s="3"/>
     </row>
     <row r="134" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A134" s="8"/>
@@ -1776,27 +1786,27 @@
       <c r="D145" s="3"/>
     </row>
     <row r="146" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A146" s="8"/>
-      <c r="B146" s="2"/>
-      <c r="C146" s="2"/>
+      <c r="A146" s="7"/>
+      <c r="B146" s="4"/>
+      <c r="C146" s="4"/>
       <c r="D146" s="3"/>
+      <c r="E146" s="4"/>
+      <c r="F146" s="3"/>
     </row>
     <row r="147" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A147" s="7"/>
-      <c r="B147" s="4"/>
-      <c r="C147" s="4"/>
+      <c r="A147" s="4"/>
+      <c r="B147" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C147" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D147" s="3"/>
-      <c r="E147" s="4"/>
-      <c r="F147" s="3"/>
     </row>
     <row r="148" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A148" s="4"/>
-      <c r="B148" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C148" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="B148" s="4"/>
+      <c r="C148" s="4"/>
       <c r="D148" s="3"/>
     </row>
     <row r="149" spans="1:6" ht="15" x14ac:dyDescent="0.25">
@@ -1983,7 +1993,6 @@
       <c r="A179" s="4"/>
       <c r="B179" s="4"/>
       <c r="C179" s="4"/>
-      <c r="D179" s="3"/>
     </row>
     <row r="180" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A180" s="4"/>
@@ -1991,7 +2000,6 @@
       <c r="C180" s="4"/>
     </row>
     <row r="181" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A181" s="4"/>
       <c r="B181" s="4"/>
       <c r="C181" s="4"/>
     </row>
@@ -2538,10 +2546,6 @@
     <row r="317" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B317" s="4"/>
       <c r="C317" s="4"/>
-    </row>
-    <row r="318" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B318" s="4"/>
-      <c r="C318" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
lowered input to 27722
</commit_message>
<xml_diff>
--- a/RallyBike/FrameCompare.xlsx
+++ b/RallyBike/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\RallyBike\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4976439-11D3-449D-874D-41C9FB0BB4F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82AB756-0159-4D41-92F4-A913DD3A6C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1101,14 +1101,14 @@
         <v>21</v>
       </c>
       <c r="B34" s="2">
-        <v>27738</v>
+        <v>27722</v>
       </c>
       <c r="C34" s="2">
         <v>31003</v>
       </c>
       <c r="D34" s="3">
         <f t="shared" ref="D34" si="1">IF(C34&lt;&gt;"",IF(B34&lt;&gt;"",C34-B34,"-"), "-")</f>
-        <v>3265</v>
+        <v>3281</v>
       </c>
       <c r="E34" s="2">
         <v>29677</v>

</xml_diff>

<commit_message>
ending input at 27700 (22 frames faster)
</commit_message>
<xml_diff>
--- a/RallyBike/FrameCompare.xlsx
+++ b/RallyBike/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\RallyBike\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82AB756-0159-4D41-92F4-A913DD3A6C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FDC68EE-9E78-4D52-8A43-22976FFAC626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1101,14 +1101,14 @@
         <v>21</v>
       </c>
       <c r="B34" s="2">
-        <v>27722</v>
+        <v>27700</v>
       </c>
       <c r="C34" s="2">
         <v>31003</v>
       </c>
       <c r="D34" s="3">
         <f t="shared" ref="D34" si="1">IF(C34&lt;&gt;"",IF(B34&lt;&gt;"",C34-B34,"-"), "-")</f>
-        <v>3281</v>
+        <v>3303</v>
       </c>
       <c r="E34" s="2">
         <v>29677</v>

</xml_diff>

<commit_message>
v4 up to race 3 end 16 frames faster by getting gas during the 2nd heli drop to spend more of the race with turbo
</commit_message>
<xml_diff>
--- a/RallyBike/FrameCompare.xlsx
+++ b/RallyBike/FrameCompare.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\RallyBike\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E461024F-440E-4570-8672-F9F53B94FCC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32989698-E7E3-489E-A9B0-6931A2BF62FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38910" yWindow="4725" windowWidth="14490" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45705" yWindow="1350" windowWidth="14490" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="V6" sheetId="10" r:id="rId1"/>
+    <sheet name="V4" sheetId="11" r:id="rId1"/>
+    <sheet name="V3" sheetId="10" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="27">
   <si>
     <t>Place</t>
   </si>
@@ -42,9 +43,6 @@
   </si>
   <si>
     <t>juef</t>
-  </si>
-  <si>
-    <t>V2</t>
   </si>
   <si>
     <t>Title screen appears</t>
@@ -99,6 +97,21 @@
   </si>
   <si>
     <t>without delying cross finish</t>
+  </si>
+  <si>
+    <t>V3</t>
+  </si>
+  <si>
+    <t>V4</t>
+  </si>
+  <si>
+    <t>Get Turbo</t>
+  </si>
+  <si>
+    <t>Get Gas</t>
+  </si>
+  <si>
+    <t>Turbo to 180</t>
   </si>
 </sst>
 </file>
@@ -247,7 +260,7 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -265,6 +278,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Accent1" xfId="5" builtinId="29"/>
@@ -584,12 +598,1992 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{315779BE-0457-4CD0-8DEA-0D00DE0D8921}">
+  <dimension ref="A1:F320"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.375" customWidth="1"/>
+    <col min="4" max="4" width="6.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3">
+        <f t="shared" ref="D2:D37" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="2">
+        <v>94</v>
+      </c>
+      <c r="C3" s="2">
+        <v>94</v>
+      </c>
+      <c r="D3" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2">
+        <v>334</v>
+      </c>
+      <c r="C4" s="2">
+        <v>334</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2294</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2294</v>
+      </c>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <v>5258</v>
+      </c>
+      <c r="C6" s="2">
+        <v>5258</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2">
+        <v>5509</v>
+      </c>
+      <c r="C7" s="2">
+        <v>5509</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2">
+        <v>5756</v>
+      </c>
+      <c r="C8" s="2">
+        <v>5756</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2">
+        <v>5775</v>
+      </c>
+      <c r="C9" s="2">
+        <v>5775</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="5">
+        <v>5796</v>
+      </c>
+      <c r="C10" s="5">
+        <v>5796</v>
+      </c>
+      <c r="D10" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="14">
+        <v>5878</v>
+      </c>
+      <c r="C11" s="14">
+        <v>5878</v>
+      </c>
+      <c r="D11" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="2">
+        <v>6118</v>
+      </c>
+      <c r="C12" s="2">
+        <v>6118</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2">
+        <v>12226</v>
+      </c>
+      <c r="C13" s="2">
+        <v>12226</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="2">
+        <v>12477</v>
+      </c>
+      <c r="C14" s="2">
+        <v>12477</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="2">
+        <v>12724</v>
+      </c>
+      <c r="C15" s="2">
+        <v>12724</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="2">
+        <v>12764</v>
+      </c>
+      <c r="C16" s="2">
+        <v>12764</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="5">
+        <v>12789</v>
+      </c>
+      <c r="C17" s="5">
+        <v>12789</v>
+      </c>
+      <c r="D17" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="2">
+        <v>12871</v>
+      </c>
+      <c r="C18" s="2">
+        <v>12871</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2">
+        <v>15625</v>
+      </c>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2">
+        <v>16200</v>
+      </c>
+      <c r="D20" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2">
+        <v>17675</v>
+      </c>
+      <c r="C21" s="2">
+        <v>17691</v>
+      </c>
+      <c r="D21" s="3">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="E21">
+        <v>17691</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="2">
+        <v>17926</v>
+      </c>
+      <c r="C22" s="2">
+        <v>17942</v>
+      </c>
+      <c r="D22" s="3">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2">
+        <v>18209</v>
+      </c>
+      <c r="D24" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5">
+        <v>18226</v>
+      </c>
+      <c r="D25" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2">
+        <v>18307</v>
+      </c>
+      <c r="D26" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2">
+        <v>18677</v>
+      </c>
+      <c r="D27" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5">
+        <v>18882</v>
+      </c>
+      <c r="D28" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2">
+        <v>18969</v>
+      </c>
+      <c r="D29" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2">
+        <v>24407</v>
+      </c>
+      <c r="D30" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2">
+        <v>24658</v>
+      </c>
+      <c r="D31" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2">
+        <v>24905</v>
+      </c>
+      <c r="D32" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2">
+        <v>24985</v>
+      </c>
+      <c r="D33" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5">
+        <v>25006</v>
+      </c>
+      <c r="D34" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2">
+        <v>25088</v>
+      </c>
+      <c r="D35" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2">
+        <v>29684</v>
+      </c>
+      <c r="D36" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2">
+        <v>27669</v>
+      </c>
+      <c r="D37" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="E37" s="2">
+        <v>29677</v>
+      </c>
+      <c r="F37" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="8"/>
+      <c r="B38" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" s="3"/>
+    </row>
+    <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="8"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="10"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="3"/>
+    </row>
+    <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="8"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="3"/>
+    </row>
+    <row r="42" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="8"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="3"/>
+    </row>
+    <row r="43" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="8"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="3"/>
+    </row>
+    <row r="44" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="8"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="3"/>
+    </row>
+    <row r="45" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="8"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="3"/>
+    </row>
+    <row r="46" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46" s="8"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="3"/>
+    </row>
+    <row r="47" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="8"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="3"/>
+    </row>
+    <row r="48" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="8"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="3"/>
+    </row>
+    <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" s="8"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="3"/>
+    </row>
+    <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A50" s="9"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="6"/>
+    </row>
+    <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A51" s="8"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="3"/>
+    </row>
+    <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A52" s="8"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="3"/>
+    </row>
+    <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" s="8"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="3"/>
+    </row>
+    <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54" s="9"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="6"/>
+    </row>
+    <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A55" s="8"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="3"/>
+    </row>
+    <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A56" s="8"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="3"/>
+    </row>
+    <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A57" s="8"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="3"/>
+    </row>
+    <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A58" s="9"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="6"/>
+    </row>
+    <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A59" s="8"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="3"/>
+    </row>
+    <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A60" s="8"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="3"/>
+    </row>
+    <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A61" s="8"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="3"/>
+    </row>
+    <row r="62" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A62" s="8"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="3"/>
+    </row>
+    <row r="63" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A63" s="8"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="3"/>
+    </row>
+    <row r="64" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A64" s="8"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="3"/>
+    </row>
+    <row r="65" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A65" s="8"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="3"/>
+    </row>
+    <row r="66" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A66" s="9"/>
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="6"/>
+    </row>
+    <row r="67" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A67" s="8"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="3"/>
+    </row>
+    <row r="68" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A68" s="8"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="3"/>
+    </row>
+    <row r="69" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A69" s="8"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="3"/>
+    </row>
+    <row r="70" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A70" s="8"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="3"/>
+    </row>
+    <row r="71" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A71" s="8"/>
+      <c r="B71" s="2"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="3"/>
+    </row>
+    <row r="72" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A72" s="8"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="3"/>
+    </row>
+    <row r="73" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A73" s="8"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="3"/>
+    </row>
+    <row r="74" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A74" s="9"/>
+      <c r="B74" s="5"/>
+      <c r="C74" s="5"/>
+      <c r="D74" s="6"/>
+    </row>
+    <row r="75" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A75" s="8"/>
+      <c r="B75" s="2"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="3"/>
+    </row>
+    <row r="76" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A76" s="8"/>
+      <c r="B76" s="2"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="3"/>
+    </row>
+    <row r="77" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A77" s="8"/>
+      <c r="B77" s="2"/>
+      <c r="C77" s="2"/>
+      <c r="D77" s="3"/>
+    </row>
+    <row r="78" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A78" s="8"/>
+      <c r="B78" s="2"/>
+      <c r="C78" s="2"/>
+      <c r="D78" s="3"/>
+    </row>
+    <row r="79" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A79" s="8"/>
+      <c r="B79" s="2"/>
+      <c r="C79" s="2"/>
+      <c r="D79" s="3"/>
+    </row>
+    <row r="80" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A80" s="8"/>
+      <c r="B80" s="2"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="3"/>
+    </row>
+    <row r="81" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A81" s="8"/>
+      <c r="B81" s="2"/>
+      <c r="C81" s="2"/>
+      <c r="D81" s="3"/>
+    </row>
+    <row r="82" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A82" s="9"/>
+      <c r="B82" s="5"/>
+      <c r="C82" s="5"/>
+      <c r="D82" s="6"/>
+    </row>
+    <row r="83" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A83" s="8"/>
+      <c r="B83" s="10"/>
+      <c r="C83" s="10"/>
+      <c r="D83" s="3"/>
+    </row>
+    <row r="84" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A84" s="8"/>
+      <c r="B84" s="2"/>
+      <c r="C84" s="2"/>
+      <c r="D84" s="3"/>
+    </row>
+    <row r="85" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A85" s="8"/>
+      <c r="B85" s="2"/>
+      <c r="C85" s="2"/>
+      <c r="D85" s="3"/>
+    </row>
+    <row r="86" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A86" s="8"/>
+      <c r="B86" s="2"/>
+      <c r="C86" s="2"/>
+      <c r="D86" s="3"/>
+    </row>
+    <row r="87" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A87" s="8"/>
+      <c r="B87" s="2"/>
+      <c r="C87" s="2"/>
+      <c r="D87" s="3"/>
+    </row>
+    <row r="88" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A88" s="8"/>
+      <c r="B88" s="2"/>
+      <c r="C88" s="2"/>
+      <c r="D88" s="3"/>
+    </row>
+    <row r="89" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A89" s="9"/>
+      <c r="B89" s="5"/>
+      <c r="C89" s="5"/>
+      <c r="D89" s="6"/>
+    </row>
+    <row r="90" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A90" s="8"/>
+      <c r="B90" s="2"/>
+      <c r="C90" s="2"/>
+      <c r="D90" s="3"/>
+    </row>
+    <row r="91" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A91" s="10"/>
+      <c r="B91" s="2"/>
+      <c r="C91" s="2"/>
+      <c r="D91" s="3"/>
+    </row>
+    <row r="92" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A92" s="10"/>
+      <c r="B92" s="2"/>
+      <c r="C92" s="2"/>
+      <c r="D92" s="3"/>
+    </row>
+    <row r="93" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A93" s="10"/>
+      <c r="B93" s="2"/>
+      <c r="C93" s="2"/>
+      <c r="D93" s="3"/>
+    </row>
+    <row r="94" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A94" s="10"/>
+      <c r="B94" s="2"/>
+      <c r="C94" s="2"/>
+      <c r="D94" s="3"/>
+    </row>
+    <row r="95" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A95" s="8"/>
+      <c r="B95" s="2"/>
+      <c r="C95" s="2"/>
+      <c r="D95" s="3"/>
+    </row>
+    <row r="96" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A96" s="9"/>
+      <c r="B96" s="5"/>
+      <c r="C96" s="5"/>
+      <c r="D96" s="6"/>
+    </row>
+    <row r="97" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A97" s="8"/>
+      <c r="B97" s="2"/>
+      <c r="C97" s="2"/>
+      <c r="D97" s="3"/>
+    </row>
+    <row r="98" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A98" s="8"/>
+      <c r="B98" s="2"/>
+      <c r="C98" s="2"/>
+      <c r="D98" s="3"/>
+    </row>
+    <row r="99" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A99" s="8"/>
+      <c r="B99" s="2"/>
+      <c r="C99" s="2"/>
+      <c r="D99" s="3"/>
+    </row>
+    <row r="100" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A100" s="8"/>
+      <c r="B100" s="2"/>
+      <c r="C100" s="2"/>
+      <c r="D100" s="3"/>
+    </row>
+    <row r="101" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A101" s="8"/>
+      <c r="B101" s="2"/>
+      <c r="C101" s="2"/>
+      <c r="D101" s="3"/>
+    </row>
+    <row r="102" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A102" s="8"/>
+      <c r="B102" s="2"/>
+      <c r="C102" s="2"/>
+      <c r="D102" s="3"/>
+    </row>
+    <row r="103" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A103" s="8"/>
+      <c r="B103" s="2"/>
+      <c r="C103" s="2"/>
+      <c r="D103" s="3"/>
+    </row>
+    <row r="104" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A104" s="9"/>
+      <c r="B104" s="5"/>
+      <c r="C104" s="5"/>
+      <c r="D104" s="6"/>
+    </row>
+    <row r="105" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A105" s="8"/>
+      <c r="B105" s="2"/>
+      <c r="C105" s="2"/>
+      <c r="D105" s="3"/>
+    </row>
+    <row r="106" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A106" s="8"/>
+      <c r="B106" s="2"/>
+      <c r="C106" s="2"/>
+      <c r="D106" s="3"/>
+    </row>
+    <row r="107" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A107" s="8"/>
+      <c r="B107" s="2"/>
+      <c r="C107" s="2"/>
+      <c r="D107" s="3"/>
+    </row>
+    <row r="108" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A108" s="10"/>
+      <c r="B108" s="2"/>
+      <c r="C108" s="2"/>
+      <c r="D108" s="3"/>
+    </row>
+    <row r="109" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A109" s="8"/>
+      <c r="B109" s="2"/>
+      <c r="C109" s="2"/>
+      <c r="D109" s="3"/>
+    </row>
+    <row r="110" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A110" s="8"/>
+      <c r="B110" s="2"/>
+      <c r="C110" s="2"/>
+      <c r="D110" s="3"/>
+    </row>
+    <row r="111" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A111" s="8"/>
+      <c r="B111" s="2"/>
+      <c r="C111" s="2"/>
+      <c r="D111" s="3"/>
+    </row>
+    <row r="112" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A112" s="8"/>
+      <c r="B112" s="2"/>
+      <c r="C112" s="2"/>
+      <c r="D112" s="3"/>
+    </row>
+    <row r="113" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A113" s="9"/>
+      <c r="B113" s="5"/>
+      <c r="C113" s="5"/>
+      <c r="D113" s="6"/>
+    </row>
+    <row r="114" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A114" s="8"/>
+      <c r="B114" s="2"/>
+      <c r="C114" s="2"/>
+      <c r="D114" s="3"/>
+    </row>
+    <row r="115" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A115" s="8"/>
+      <c r="B115" s="2"/>
+      <c r="C115" s="2"/>
+      <c r="D115" s="3"/>
+    </row>
+    <row r="116" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A116" s="8"/>
+      <c r="B116" s="2"/>
+      <c r="C116" s="2"/>
+      <c r="D116" s="3"/>
+    </row>
+    <row r="117" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A117" s="8"/>
+      <c r="B117" s="2"/>
+      <c r="C117" s="2"/>
+      <c r="D117" s="3"/>
+    </row>
+    <row r="118" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A118" s="8"/>
+      <c r="B118" s="2"/>
+      <c r="C118" s="2"/>
+      <c r="D118" s="3"/>
+    </row>
+    <row r="119" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A119" s="8"/>
+      <c r="B119" s="2"/>
+      <c r="C119" s="2"/>
+      <c r="D119" s="3"/>
+    </row>
+    <row r="120" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A120" s="8"/>
+      <c r="B120" s="2"/>
+      <c r="C120" s="2"/>
+      <c r="D120" s="3"/>
+    </row>
+    <row r="121" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A121" s="8"/>
+      <c r="B121" s="2"/>
+      <c r="C121" s="2"/>
+      <c r="D121" s="3"/>
+    </row>
+    <row r="122" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A122" s="8"/>
+      <c r="B122" s="2"/>
+      <c r="C122" s="2"/>
+      <c r="D122" s="3"/>
+    </row>
+    <row r="123" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A123" s="8"/>
+      <c r="B123" s="2"/>
+      <c r="C123" s="2"/>
+      <c r="D123" s="3"/>
+    </row>
+    <row r="124" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A124" s="8"/>
+      <c r="B124" s="2"/>
+      <c r="C124" s="2"/>
+      <c r="D124" s="3"/>
+    </row>
+    <row r="125" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A125" s="9"/>
+      <c r="B125" s="5"/>
+      <c r="C125" s="5"/>
+      <c r="D125" s="6"/>
+    </row>
+    <row r="126" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A126" s="8"/>
+      <c r="B126" s="2"/>
+      <c r="C126" s="2"/>
+      <c r="D126" s="3"/>
+    </row>
+    <row r="127" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A127" s="8"/>
+      <c r="B127" s="2"/>
+      <c r="C127" s="2"/>
+      <c r="D127" s="3"/>
+    </row>
+    <row r="128" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A128" s="8"/>
+      <c r="B128" s="2"/>
+      <c r="C128" s="2"/>
+      <c r="D128" s="3"/>
+    </row>
+    <row r="129" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A129" s="8"/>
+      <c r="B129" s="2"/>
+      <c r="C129" s="2"/>
+      <c r="D129" s="3"/>
+    </row>
+    <row r="130" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A130" s="8"/>
+      <c r="B130" s="2"/>
+      <c r="C130" s="2"/>
+      <c r="D130" s="3"/>
+    </row>
+    <row r="131" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A131" s="8"/>
+      <c r="B131" s="2"/>
+      <c r="C131" s="2"/>
+      <c r="D131" s="3"/>
+    </row>
+    <row r="132" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A132" s="8"/>
+      <c r="B132" s="2"/>
+      <c r="C132" s="2"/>
+      <c r="D132" s="3"/>
+    </row>
+    <row r="133" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A133" s="8"/>
+      <c r="B133" s="2"/>
+      <c r="C133" s="2"/>
+      <c r="D133" s="3"/>
+    </row>
+    <row r="134" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A134" s="8"/>
+      <c r="B134" s="2"/>
+      <c r="C134" s="2"/>
+      <c r="D134" s="3"/>
+    </row>
+    <row r="135" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A135" s="9"/>
+      <c r="B135" s="5"/>
+      <c r="C135" s="5"/>
+      <c r="D135" s="6"/>
+    </row>
+    <row r="136" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A136" s="8"/>
+      <c r="B136" s="2"/>
+      <c r="C136" s="2"/>
+      <c r="D136" s="3"/>
+    </row>
+    <row r="137" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A137" s="8"/>
+      <c r="B137" s="2"/>
+      <c r="C137" s="2"/>
+      <c r="D137" s="3"/>
+    </row>
+    <row r="138" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A138" s="8"/>
+      <c r="B138" s="2"/>
+      <c r="C138" s="2"/>
+      <c r="D138" s="3"/>
+    </row>
+    <row r="139" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A139" s="8"/>
+      <c r="B139" s="2"/>
+      <c r="C139" s="2"/>
+      <c r="D139" s="3"/>
+    </row>
+    <row r="140" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A140" s="8"/>
+      <c r="B140" s="2"/>
+      <c r="C140" s="2"/>
+      <c r="D140" s="3"/>
+    </row>
+    <row r="141" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A141" s="8"/>
+      <c r="B141" s="2"/>
+      <c r="C141" s="2"/>
+      <c r="D141" s="3"/>
+    </row>
+    <row r="142" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A142" s="8"/>
+      <c r="B142" s="2"/>
+      <c r="C142" s="2"/>
+      <c r="D142" s="3"/>
+    </row>
+    <row r="143" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A143" s="8"/>
+      <c r="B143" s="2"/>
+      <c r="C143" s="2"/>
+      <c r="D143" s="3"/>
+    </row>
+    <row r="144" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A144" s="8"/>
+      <c r="B144" s="2"/>
+      <c r="C144" s="2"/>
+      <c r="D144" s="3"/>
+    </row>
+    <row r="145" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A145" s="8"/>
+      <c r="B145" s="2"/>
+      <c r="C145" s="2"/>
+      <c r="D145" s="3"/>
+    </row>
+    <row r="146" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A146" s="8"/>
+      <c r="B146" s="2"/>
+      <c r="C146" s="2"/>
+      <c r="D146" s="3"/>
+    </row>
+    <row r="147" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A147" s="8"/>
+      <c r="B147" s="2"/>
+      <c r="C147" s="2"/>
+      <c r="D147" s="3"/>
+    </row>
+    <row r="148" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A148" s="8"/>
+      <c r="B148" s="2"/>
+      <c r="C148" s="2"/>
+      <c r="D148" s="3"/>
+    </row>
+    <row r="149" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A149" s="7"/>
+      <c r="B149" s="4"/>
+      <c r="C149" s="4"/>
+      <c r="D149" s="3"/>
+      <c r="E149" s="4"/>
+      <c r="F149" s="3"/>
+    </row>
+    <row r="150" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A150" s="4"/>
+      <c r="B150" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C150" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D150" s="3"/>
+    </row>
+    <row r="151" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A151" s="4"/>
+      <c r="B151" s="4"/>
+      <c r="C151" s="4"/>
+      <c r="D151" s="3"/>
+    </row>
+    <row r="152" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A152" s="4"/>
+      <c r="B152" s="4"/>
+      <c r="C152" s="4"/>
+      <c r="D152" s="3"/>
+    </row>
+    <row r="153" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A153" s="4"/>
+      <c r="B153" s="4"/>
+      <c r="C153" s="4"/>
+      <c r="D153" s="3"/>
+    </row>
+    <row r="154" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A154" s="4"/>
+      <c r="B154" s="4"/>
+      <c r="C154" s="4"/>
+      <c r="D154" s="3"/>
+    </row>
+    <row r="155" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A155" s="4"/>
+      <c r="B155" s="4"/>
+      <c r="C155" s="4"/>
+      <c r="D155" s="3"/>
+    </row>
+    <row r="156" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A156" s="4"/>
+      <c r="B156" s="4"/>
+      <c r="C156" s="4"/>
+      <c r="D156" s="3"/>
+    </row>
+    <row r="157" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A157" s="4"/>
+      <c r="B157" s="4"/>
+      <c r="C157" s="4"/>
+      <c r="D157" s="3"/>
+    </row>
+    <row r="158" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A158" s="4"/>
+      <c r="B158" s="4"/>
+      <c r="C158" s="4"/>
+      <c r="D158" s="3"/>
+    </row>
+    <row r="159" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A159" s="4"/>
+      <c r="B159" s="4"/>
+      <c r="C159" s="4"/>
+      <c r="D159" s="3"/>
+    </row>
+    <row r="160" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A160" s="4"/>
+      <c r="B160" s="4"/>
+      <c r="C160" s="4"/>
+      <c r="D160" s="3"/>
+    </row>
+    <row r="161" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A161" s="4"/>
+      <c r="B161" s="4"/>
+      <c r="C161" s="4"/>
+      <c r="D161" s="3"/>
+    </row>
+    <row r="162" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A162" s="4"/>
+      <c r="B162" s="4"/>
+      <c r="C162" s="4"/>
+      <c r="D162" s="3"/>
+    </row>
+    <row r="163" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A163" s="4"/>
+      <c r="B163" s="4"/>
+      <c r="C163" s="4"/>
+      <c r="D163" s="3"/>
+    </row>
+    <row r="164" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A164" s="4"/>
+      <c r="B164" s="4"/>
+      <c r="C164" s="4"/>
+      <c r="D164" s="3"/>
+    </row>
+    <row r="165" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A165" s="4"/>
+      <c r="B165" s="4"/>
+      <c r="C165" s="4"/>
+      <c r="D165" s="3"/>
+    </row>
+    <row r="166" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A166" s="4"/>
+      <c r="B166" s="4"/>
+      <c r="C166" s="4"/>
+      <c r="D166" s="3"/>
+    </row>
+    <row r="167" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A167" s="4"/>
+      <c r="B167" s="4"/>
+      <c r="C167" s="4"/>
+      <c r="D167" s="3"/>
+    </row>
+    <row r="168" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A168" s="4"/>
+      <c r="B168" s="4"/>
+      <c r="C168" s="4"/>
+      <c r="D168" s="3"/>
+    </row>
+    <row r="169" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A169" s="4"/>
+      <c r="B169" s="4"/>
+      <c r="C169" s="4"/>
+      <c r="D169" s="3"/>
+    </row>
+    <row r="170" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A170" s="4"/>
+      <c r="B170" s="4"/>
+      <c r="C170" s="4"/>
+      <c r="D170" s="3"/>
+    </row>
+    <row r="171" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A171" s="4"/>
+      <c r="B171" s="4"/>
+      <c r="C171" s="4"/>
+      <c r="D171" s="3"/>
+    </row>
+    <row r="172" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A172" s="4"/>
+      <c r="B172" s="4"/>
+      <c r="C172" s="4"/>
+      <c r="D172" s="3"/>
+    </row>
+    <row r="173" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A173" s="4"/>
+      <c r="B173" s="4"/>
+      <c r="C173" s="4"/>
+      <c r="D173" s="3"/>
+    </row>
+    <row r="174" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A174" s="4"/>
+      <c r="B174" s="4"/>
+      <c r="C174" s="4"/>
+      <c r="D174" s="3"/>
+    </row>
+    <row r="175" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A175" s="4"/>
+      <c r="B175" s="4"/>
+      <c r="C175" s="4"/>
+      <c r="D175" s="3"/>
+    </row>
+    <row r="176" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A176" s="4"/>
+      <c r="B176" s="4"/>
+      <c r="C176" s="4"/>
+      <c r="D176" s="3"/>
+    </row>
+    <row r="177" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A177" s="4"/>
+      <c r="B177" s="4"/>
+      <c r="C177" s="4"/>
+      <c r="D177" s="3"/>
+    </row>
+    <row r="178" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A178" s="4"/>
+      <c r="B178" s="4"/>
+      <c r="C178" s="4"/>
+      <c r="D178" s="3"/>
+    </row>
+    <row r="179" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A179" s="4"/>
+      <c r="B179" s="4"/>
+      <c r="C179" s="4"/>
+      <c r="D179" s="3"/>
+    </row>
+    <row r="180" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A180" s="4"/>
+      <c r="B180" s="4"/>
+      <c r="C180" s="4"/>
+      <c r="D180" s="3"/>
+    </row>
+    <row r="181" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A181" s="4"/>
+      <c r="B181" s="4"/>
+      <c r="C181" s="4"/>
+      <c r="D181" s="3"/>
+    </row>
+    <row r="182" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A182" s="4"/>
+      <c r="B182" s="4"/>
+      <c r="C182" s="4"/>
+    </row>
+    <row r="183" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A183" s="4"/>
+      <c r="B183" s="4"/>
+      <c r="C183" s="4"/>
+    </row>
+    <row r="184" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B184" s="4"/>
+      <c r="C184" s="4"/>
+    </row>
+    <row r="185" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B185" s="4"/>
+      <c r="C185" s="4"/>
+    </row>
+    <row r="186" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B186" s="4"/>
+      <c r="C186" s="4"/>
+    </row>
+    <row r="187" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B187" s="4"/>
+      <c r="C187" s="4"/>
+    </row>
+    <row r="188" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B188" s="4"/>
+      <c r="C188" s="4"/>
+    </row>
+    <row r="189" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B189" s="4"/>
+      <c r="C189" s="4"/>
+    </row>
+    <row r="190" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B190" s="4"/>
+      <c r="C190" s="4"/>
+    </row>
+    <row r="191" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B191" s="4"/>
+      <c r="C191" s="4"/>
+    </row>
+    <row r="192" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B192" s="4"/>
+      <c r="C192" s="4"/>
+    </row>
+    <row r="193" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B193" s="4"/>
+      <c r="C193" s="4"/>
+    </row>
+    <row r="194" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B194" s="4"/>
+      <c r="C194" s="4"/>
+    </row>
+    <row r="195" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B195" s="4"/>
+      <c r="C195" s="4"/>
+    </row>
+    <row r="196" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B196" s="4"/>
+      <c r="C196" s="4"/>
+    </row>
+    <row r="197" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B197" s="4"/>
+      <c r="C197" s="4"/>
+    </row>
+    <row r="198" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B198" s="4"/>
+      <c r="C198" s="4"/>
+    </row>
+    <row r="199" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B199" s="4"/>
+      <c r="C199" s="4"/>
+    </row>
+    <row r="200" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B200" s="4"/>
+      <c r="C200" s="4"/>
+    </row>
+    <row r="201" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B201" s="4"/>
+      <c r="C201" s="4"/>
+    </row>
+    <row r="202" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B202" s="4"/>
+      <c r="C202" s="4"/>
+    </row>
+    <row r="203" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B203" s="4"/>
+      <c r="C203" s="4"/>
+    </row>
+    <row r="204" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B204" s="4"/>
+      <c r="C204" s="4"/>
+    </row>
+    <row r="205" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B205" s="4"/>
+      <c r="C205" s="4"/>
+    </row>
+    <row r="206" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B206" s="4"/>
+      <c r="C206" s="4"/>
+    </row>
+    <row r="207" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B207" s="4"/>
+      <c r="C207" s="4"/>
+    </row>
+    <row r="208" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B208" s="4"/>
+      <c r="C208" s="4"/>
+    </row>
+    <row r="209" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B209" s="4"/>
+      <c r="C209" s="4"/>
+    </row>
+    <row r="210" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B210" s="4"/>
+      <c r="C210" s="4"/>
+    </row>
+    <row r="211" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B211" s="4"/>
+      <c r="C211" s="4"/>
+    </row>
+    <row r="212" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B212" s="4"/>
+      <c r="C212" s="4"/>
+    </row>
+    <row r="213" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B213" s="4"/>
+      <c r="C213" s="4"/>
+    </row>
+    <row r="214" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B214" s="4"/>
+      <c r="C214" s="4"/>
+    </row>
+    <row r="215" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B215" s="4"/>
+      <c r="C215" s="4"/>
+    </row>
+    <row r="216" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B216" s="4"/>
+      <c r="C216" s="4"/>
+    </row>
+    <row r="217" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B217" s="4"/>
+      <c r="C217" s="4"/>
+    </row>
+    <row r="218" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B218" s="4"/>
+      <c r="C218" s="4"/>
+    </row>
+    <row r="219" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B219" s="4"/>
+      <c r="C219" s="4"/>
+    </row>
+    <row r="220" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B220" s="4"/>
+      <c r="C220" s="4"/>
+    </row>
+    <row r="221" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B221" s="4"/>
+      <c r="C221" s="4"/>
+    </row>
+    <row r="222" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B222" s="4"/>
+      <c r="C222" s="4"/>
+    </row>
+    <row r="223" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B223" s="4"/>
+      <c r="C223" s="4"/>
+    </row>
+    <row r="224" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B224" s="4"/>
+      <c r="C224" s="4"/>
+    </row>
+    <row r="225" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B225" s="4"/>
+      <c r="C225" s="4"/>
+    </row>
+    <row r="226" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B226" s="4"/>
+      <c r="C226" s="4"/>
+    </row>
+    <row r="227" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B227" s="4"/>
+      <c r="C227" s="4"/>
+    </row>
+    <row r="228" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B228" s="4"/>
+      <c r="C228" s="4"/>
+    </row>
+    <row r="229" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B229" s="4"/>
+      <c r="C229" s="4"/>
+    </row>
+    <row r="230" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B230" s="4"/>
+      <c r="C230" s="4"/>
+    </row>
+    <row r="231" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B231" s="4"/>
+      <c r="C231" s="4"/>
+    </row>
+    <row r="232" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B232" s="4"/>
+      <c r="C232" s="4"/>
+    </row>
+    <row r="233" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B233" s="4"/>
+      <c r="C233" s="4"/>
+    </row>
+    <row r="234" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B234" s="4"/>
+      <c r="C234" s="4"/>
+    </row>
+    <row r="235" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B235" s="4"/>
+      <c r="C235" s="4"/>
+    </row>
+    <row r="236" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B236" s="4"/>
+      <c r="C236" s="4"/>
+    </row>
+    <row r="237" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B237" s="4"/>
+      <c r="C237" s="4"/>
+    </row>
+    <row r="238" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B238" s="4"/>
+      <c r="C238" s="4"/>
+    </row>
+    <row r="239" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B239" s="4"/>
+      <c r="C239" s="4"/>
+    </row>
+    <row r="240" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B240" s="4"/>
+      <c r="C240" s="4"/>
+    </row>
+    <row r="241" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B241" s="4"/>
+      <c r="C241" s="4"/>
+    </row>
+    <row r="242" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B242" s="4"/>
+      <c r="C242" s="4"/>
+    </row>
+    <row r="243" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B243" s="4"/>
+      <c r="C243" s="4"/>
+    </row>
+    <row r="244" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B244" s="4"/>
+      <c r="C244" s="4"/>
+    </row>
+    <row r="245" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B245" s="4"/>
+      <c r="C245" s="4"/>
+    </row>
+    <row r="246" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B246" s="4"/>
+      <c r="C246" s="4"/>
+    </row>
+    <row r="247" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B247" s="4"/>
+      <c r="C247" s="4"/>
+    </row>
+    <row r="248" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B248" s="4"/>
+      <c r="C248" s="4"/>
+    </row>
+    <row r="249" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B249" s="4"/>
+      <c r="C249" s="4"/>
+    </row>
+    <row r="250" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B250" s="4"/>
+      <c r="C250" s="4"/>
+    </row>
+    <row r="251" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B251" s="4"/>
+      <c r="C251" s="4"/>
+    </row>
+    <row r="252" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B252" s="4"/>
+      <c r="C252" s="4"/>
+    </row>
+    <row r="253" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B253" s="4"/>
+      <c r="C253" s="4"/>
+    </row>
+    <row r="254" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B254" s="4"/>
+      <c r="C254" s="4"/>
+    </row>
+    <row r="255" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B255" s="4"/>
+      <c r="C255" s="4"/>
+    </row>
+    <row r="256" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B256" s="4"/>
+      <c r="C256" s="4"/>
+    </row>
+    <row r="257" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B257" s="4"/>
+      <c r="C257" s="4"/>
+    </row>
+    <row r="258" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B258" s="4"/>
+      <c r="C258" s="4"/>
+    </row>
+    <row r="259" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B259" s="4"/>
+      <c r="C259" s="4"/>
+    </row>
+    <row r="260" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B260" s="4"/>
+      <c r="C260" s="4"/>
+    </row>
+    <row r="261" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B261" s="4"/>
+      <c r="C261" s="4"/>
+    </row>
+    <row r="262" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B262" s="4"/>
+      <c r="C262" s="4"/>
+    </row>
+    <row r="263" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B263" s="4"/>
+      <c r="C263" s="4"/>
+    </row>
+    <row r="264" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B264" s="4"/>
+      <c r="C264" s="4"/>
+    </row>
+    <row r="265" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B265" s="4"/>
+      <c r="C265" s="4"/>
+    </row>
+    <row r="266" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B266" s="4"/>
+      <c r="C266" s="4"/>
+    </row>
+    <row r="267" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B267" s="4"/>
+      <c r="C267" s="4"/>
+    </row>
+    <row r="268" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B268" s="4"/>
+      <c r="C268" s="4"/>
+    </row>
+    <row r="269" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B269" s="4"/>
+      <c r="C269" s="4"/>
+    </row>
+    <row r="270" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B270" s="4"/>
+      <c r="C270" s="4"/>
+    </row>
+    <row r="271" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B271" s="4"/>
+      <c r="C271" s="4"/>
+    </row>
+    <row r="272" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B272" s="4"/>
+      <c r="C272" s="4"/>
+    </row>
+    <row r="273" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B273" s="4"/>
+      <c r="C273" s="4"/>
+    </row>
+    <row r="274" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B274" s="4"/>
+      <c r="C274" s="4"/>
+    </row>
+    <row r="275" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B275" s="4"/>
+      <c r="C275" s="4"/>
+    </row>
+    <row r="276" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B276" s="4"/>
+      <c r="C276" s="4"/>
+    </row>
+    <row r="277" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B277" s="4"/>
+      <c r="C277" s="4"/>
+    </row>
+    <row r="278" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B278" s="4"/>
+      <c r="C278" s="4"/>
+    </row>
+    <row r="279" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B279" s="4"/>
+      <c r="C279" s="4"/>
+    </row>
+    <row r="280" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B280" s="4"/>
+      <c r="C280" s="4"/>
+    </row>
+    <row r="281" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B281" s="4"/>
+      <c r="C281" s="4"/>
+    </row>
+    <row r="282" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B282" s="4"/>
+      <c r="C282" s="4"/>
+    </row>
+    <row r="283" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B283" s="4"/>
+      <c r="C283" s="4"/>
+    </row>
+    <row r="284" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B284" s="4"/>
+      <c r="C284" s="4"/>
+    </row>
+    <row r="285" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B285" s="4"/>
+      <c r="C285" s="4"/>
+    </row>
+    <row r="286" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B286" s="4"/>
+      <c r="C286" s="4"/>
+    </row>
+    <row r="287" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B287" s="4"/>
+      <c r="C287" s="4"/>
+    </row>
+    <row r="288" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B288" s="4"/>
+      <c r="C288" s="4"/>
+    </row>
+    <row r="289" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B289" s="4"/>
+      <c r="C289" s="4"/>
+    </row>
+    <row r="290" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B290" s="4"/>
+      <c r="C290" s="4"/>
+    </row>
+    <row r="291" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B291" s="4"/>
+      <c r="C291" s="4"/>
+    </row>
+    <row r="292" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B292" s="4"/>
+      <c r="C292" s="4"/>
+    </row>
+    <row r="293" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B293" s="4"/>
+      <c r="C293" s="4"/>
+    </row>
+    <row r="294" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B294" s="4"/>
+      <c r="C294" s="4"/>
+    </row>
+    <row r="295" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B295" s="4"/>
+      <c r="C295" s="4"/>
+    </row>
+    <row r="296" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B296" s="4"/>
+      <c r="C296" s="4"/>
+    </row>
+    <row r="297" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B297" s="4"/>
+      <c r="C297" s="4"/>
+    </row>
+    <row r="298" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B298" s="4"/>
+      <c r="C298" s="4"/>
+    </row>
+    <row r="299" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B299" s="4"/>
+      <c r="C299" s="4"/>
+    </row>
+    <row r="300" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B300" s="4"/>
+      <c r="C300" s="4"/>
+    </row>
+    <row r="301" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B301" s="4"/>
+      <c r="C301" s="4"/>
+    </row>
+    <row r="302" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B302" s="4"/>
+      <c r="C302" s="4"/>
+    </row>
+    <row r="303" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B303" s="4"/>
+      <c r="C303" s="4"/>
+    </row>
+    <row r="304" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B304" s="4"/>
+      <c r="C304" s="4"/>
+    </row>
+    <row r="305" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B305" s="4"/>
+      <c r="C305" s="4"/>
+    </row>
+    <row r="306" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B306" s="4"/>
+      <c r="C306" s="4"/>
+    </row>
+    <row r="307" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B307" s="4"/>
+      <c r="C307" s="4"/>
+    </row>
+    <row r="308" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B308" s="4"/>
+      <c r="C308" s="4"/>
+    </row>
+    <row r="309" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B309" s="4"/>
+      <c r="C309" s="4"/>
+    </row>
+    <row r="310" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B310" s="4"/>
+      <c r="C310" s="4"/>
+    </row>
+    <row r="311" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B311" s="4"/>
+      <c r="C311" s="4"/>
+    </row>
+    <row r="312" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B312" s="4"/>
+      <c r="C312" s="4"/>
+    </row>
+    <row r="313" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B313" s="4"/>
+      <c r="C313" s="4"/>
+    </row>
+    <row r="314" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B314" s="4"/>
+      <c r="C314" s="4"/>
+    </row>
+    <row r="315" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B315" s="4"/>
+      <c r="C315" s="4"/>
+    </row>
+    <row r="316" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B316" s="4"/>
+      <c r="C316" s="4"/>
+    </row>
+    <row r="317" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B317" s="4"/>
+      <c r="C317" s="4"/>
+    </row>
+    <row r="318" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B318" s="4"/>
+      <c r="C318" s="4"/>
+    </row>
+    <row r="319" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B319" s="4"/>
+      <c r="C319" s="4"/>
+    </row>
+    <row r="320" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B320" s="4"/>
+      <c r="C320" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E7E52CC-3356-4254-B5E7-E1B0B655F38D}">
   <dimension ref="A1:F317"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -605,7 +2599,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -616,7 +2610,7 @@
     </row>
     <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2">
         <v>10</v>
@@ -632,7 +2626,7 @@
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2">
         <v>94</v>
@@ -648,7 +2642,7 @@
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2">
         <v>334</v>
@@ -663,7 +2657,7 @@
     </row>
     <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2">
         <v>5258</v>
@@ -678,7 +2672,7 @@
     </row>
     <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2">
         <v>5509</v>
@@ -693,7 +2687,7 @@
     </row>
     <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2">
         <v>5756</v>
@@ -708,7 +2702,7 @@
     </row>
     <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2">
         <v>5775</v>
@@ -723,7 +2717,7 @@
     </row>
     <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="5">
         <v>5796</v>
@@ -736,12 +2730,12 @@
         <v>50</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="14">
         <v>5878</v>
@@ -756,7 +2750,7 @@
     </row>
     <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" s="2">
         <v>6118</v>
@@ -771,7 +2765,7 @@
     </row>
     <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" s="2">
         <v>12226</v>
@@ -784,12 +2778,12 @@
         <v>50</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" s="2">
         <v>12477</v>
@@ -804,7 +2798,7 @@
     </row>
     <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" s="2">
         <v>12724</v>
@@ -819,7 +2813,7 @@
     </row>
     <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15" s="2">
         <v>12764</v>
@@ -834,7 +2828,7 @@
     </row>
     <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16" s="5">
         <v>12789</v>
@@ -849,7 +2843,7 @@
     </row>
     <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" s="2">
         <v>12871</v>
@@ -864,7 +2858,7 @@
     </row>
     <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B18" s="2">
         <v>17691</v>
@@ -882,7 +2876,7 @@
     </row>
     <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B19" s="2">
         <v>17942</v>
@@ -895,7 +2889,7 @@
     </row>
     <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -903,7 +2897,7 @@
     </row>
     <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B21" s="2">
         <v>18209</v>
@@ -918,7 +2912,7 @@
     </row>
     <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B22" s="5">
         <v>18226</v>
@@ -933,7 +2927,7 @@
     </row>
     <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" s="2">
         <v>18307</v>
@@ -948,7 +2942,7 @@
     </row>
     <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B24" s="2">
         <v>18677</v>
@@ -963,7 +2957,7 @@
     </row>
     <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B25" s="5">
         <v>18882</v>
@@ -978,7 +2972,7 @@
     </row>
     <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B26" s="2">
         <v>18969</v>
@@ -993,7 +2987,7 @@
     </row>
     <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B27" s="2">
         <v>24407</v>
@@ -1008,7 +3002,7 @@
     </row>
     <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B28" s="2">
         <v>24658</v>
@@ -1023,7 +3017,7 @@
     </row>
     <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B29" s="2">
         <v>24905</v>
@@ -1038,7 +3032,7 @@
     </row>
     <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B30" s="2">
         <v>24985</v>
@@ -1053,7 +3047,7 @@
     </row>
     <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B31" s="5">
         <v>25006</v>
@@ -1068,7 +3062,7 @@
     </row>
     <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B32" s="2">
         <v>25088</v>
@@ -1083,7 +3077,7 @@
     </row>
     <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B33" s="2">
         <v>29684</v>
@@ -1098,7 +3092,7 @@
     </row>
     <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B34" s="2">
         <v>27669</v>
@@ -1114,7 +3108,7 @@
         <v>29677</v>
       </c>
       <c r="F34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
race 3 2 frames faster
</commit_message>
<xml_diff>
--- a/RallyBike/FrameCompare.xlsx
+++ b/RallyBike/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\RallyBike\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32989698-E7E3-489E-A9B0-6931A2BF62FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FE53DC-9FC9-4BFE-9DC2-C75A3332DCE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45705" yWindow="1350" windowWidth="14490" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="28">
   <si>
     <t>Place</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>Turbo to 180</t>
+  </si>
+  <si>
+    <t>Turbo 180</t>
   </si>
 </sst>
 </file>
@@ -599,11 +602,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{315779BE-0457-4CD0-8DEA-0D00DE0D8921}">
-  <dimension ref="A1:F320"/>
+  <dimension ref="A1:F321"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -638,7 +641,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="3">
-        <f t="shared" ref="D2:D37" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
+        <f t="shared" ref="D2:D38" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
         <v>0</v>
       </c>
       <c r="F2" s="2"/>
@@ -901,141 +904,140 @@
       <c r="A20" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" s="2">
+        <v>15514</v>
+      </c>
       <c r="C20" s="2">
         <v>16200</v>
       </c>
-      <c r="D20" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D20" s="3">
+        <f t="shared" si="0"/>
+        <v>686</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>6</v>
+      <c r="A21" s="17" t="s">
+        <v>27</v>
       </c>
       <c r="B21" s="2">
-        <v>17675</v>
-      </c>
-      <c r="C21" s="2">
-        <v>17691</v>
-      </c>
-      <c r="D21" s="3">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="E21">
-        <v>17691</v>
-      </c>
+        <v>15905</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B22" s="2">
-        <v>17926</v>
+        <v>17673</v>
       </c>
       <c r="C22" s="2">
-        <v>17942</v>
+        <v>17691</v>
       </c>
       <c r="D22" s="3">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="E22">
+        <v>17691</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="3"/>
+        <v>7</v>
+      </c>
+      <c r="B23" s="2">
+        <v>17924</v>
+      </c>
+      <c r="C23" s="2">
+        <v>17942</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
     </row>
     <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2">
         <v>18209</v>
       </c>
-      <c r="D24" s="3" t="str">
+      <c r="D25" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
+    <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5">
+      <c r="B26" s="5"/>
+      <c r="C26" s="5">
         <v>18226</v>
       </c>
-      <c r="D25" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2">
-        <v>18307</v>
-      </c>
-      <c r="D26" s="3" t="str">
+      <c r="D26" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2">
+        <v>18307</v>
+      </c>
+      <c r="D27" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2">
         <v>18677</v>
       </c>
-      <c r="D27" s="3" t="str">
+      <c r="D28" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
+    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5">
+      <c r="B29" s="5"/>
+      <c r="C29" s="5">
         <v>18882</v>
       </c>
-      <c r="D28" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2">
-        <v>18969</v>
-      </c>
-      <c r="D29" s="3" t="str">
+      <c r="D29" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2">
-        <v>24407</v>
+        <v>18969</v>
       </c>
       <c r="D30" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1044,11 +1046,11 @@
     </row>
     <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2">
-        <v>24658</v>
+        <v>24407</v>
       </c>
       <c r="D31" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1057,11 +1059,11 @@
     </row>
     <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2">
-        <v>24905</v>
+        <v>24658</v>
       </c>
       <c r="D32" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1070,50 +1072,50 @@
     </row>
     <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2">
+        <v>24905</v>
+      </c>
+      <c r="D33" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2">
         <v>24985</v>
       </c>
-      <c r="D33" s="3" t="str">
+      <c r="D34" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="12" t="s">
+    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5">
+      <c r="B35" s="5"/>
+      <c r="C35" s="5">
         <v>25006</v>
       </c>
-      <c r="D34" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2">
-        <v>25088</v>
-      </c>
-      <c r="D35" s="3" t="str">
+      <c r="D35" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2">
-        <v>29684</v>
+        <v>25088</v>
       </c>
       <c r="D36" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1122,47 +1124,54 @@
     </row>
     <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2">
+        <v>29684</v>
+      </c>
+      <c r="D37" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2">
         <v>27669</v>
       </c>
-      <c r="D37" s="3" t="str">
+      <c r="D38" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E37" s="2">
+      <c r="E38" s="2">
         <v>29677</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F38" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="8"/>
-      <c r="B38" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="C38" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="D38" s="3"/>
     </row>
     <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
+      <c r="B39" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>2</v>
+      </c>
       <c r="D39" s="3"/>
     </row>
     <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="10"/>
+      <c r="A40" s="8"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="3"/>
     </row>
     <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="8"/>
+      <c r="A41" s="10"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="3"/>
@@ -1216,16 +1225,16 @@
       <c r="D49" s="3"/>
     </row>
     <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A50" s="9"/>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="6"/>
+      <c r="A50" s="8"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="3"/>
     </row>
     <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="8"/>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="3"/>
+      <c r="A51" s="9"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="6"/>
     </row>
     <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="8"/>
@@ -1240,16 +1249,16 @@
       <c r="D53" s="3"/>
     </row>
     <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A54" s="9"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="6"/>
+      <c r="A54" s="8"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="3"/>
     </row>
     <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A55" s="8"/>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="3"/>
+      <c r="A55" s="9"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="6"/>
     </row>
     <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="8"/>
@@ -1264,16 +1273,16 @@
       <c r="D57" s="3"/>
     </row>
     <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A58" s="9"/>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="6"/>
+      <c r="A58" s="8"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="3"/>
     </row>
     <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A59" s="8"/>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="3"/>
+      <c r="A59" s="9"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="6"/>
     </row>
     <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="8"/>
@@ -1312,16 +1321,16 @@
       <c r="D65" s="3"/>
     </row>
     <row r="66" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A66" s="9"/>
-      <c r="B66" s="5"/>
-      <c r="C66" s="5"/>
-      <c r="D66" s="6"/>
+      <c r="A66" s="8"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="3"/>
     </row>
     <row r="67" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A67" s="8"/>
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="3"/>
+      <c r="A67" s="9"/>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="6"/>
     </row>
     <row r="68" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="8"/>
@@ -1360,16 +1369,16 @@
       <c r="D73" s="3"/>
     </row>
     <row r="74" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A74" s="9"/>
-      <c r="B74" s="5"/>
-      <c r="C74" s="5"/>
-      <c r="D74" s="6"/>
+      <c r="A74" s="8"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="3"/>
     </row>
     <row r="75" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A75" s="8"/>
-      <c r="B75" s="2"/>
-      <c r="C75" s="2"/>
-      <c r="D75" s="3"/>
+      <c r="A75" s="9"/>
+      <c r="B75" s="5"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="6"/>
     </row>
     <row r="76" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="8"/>
@@ -1408,21 +1417,21 @@
       <c r="D81" s="3"/>
     </row>
     <row r="82" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A82" s="9"/>
-      <c r="B82" s="5"/>
-      <c r="C82" s="5"/>
-      <c r="D82" s="6"/>
+      <c r="A82" s="8"/>
+      <c r="B82" s="2"/>
+      <c r="C82" s="2"/>
+      <c r="D82" s="3"/>
     </row>
     <row r="83" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A83" s="8"/>
-      <c r="B83" s="10"/>
-      <c r="C83" s="10"/>
-      <c r="D83" s="3"/>
+      <c r="A83" s="9"/>
+      <c r="B83" s="5"/>
+      <c r="C83" s="5"/>
+      <c r="D83" s="6"/>
     </row>
     <row r="84" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="8"/>
-      <c r="B84" s="2"/>
-      <c r="C84" s="2"/>
+      <c r="B84" s="10"/>
+      <c r="C84" s="10"/>
       <c r="D84" s="3"/>
     </row>
     <row r="85" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -1450,19 +1459,19 @@
       <c r="D88" s="3"/>
     </row>
     <row r="89" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A89" s="9"/>
-      <c r="B89" s="5"/>
-      <c r="C89" s="5"/>
-      <c r="D89" s="6"/>
+      <c r="A89" s="8"/>
+      <c r="B89" s="2"/>
+      <c r="C89" s="2"/>
+      <c r="D89" s="3"/>
     </row>
     <row r="90" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A90" s="8"/>
-      <c r="B90" s="2"/>
-      <c r="C90" s="2"/>
-      <c r="D90" s="3"/>
+      <c r="A90" s="9"/>
+      <c r="B90" s="5"/>
+      <c r="C90" s="5"/>
+      <c r="D90" s="6"/>
     </row>
     <row r="91" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A91" s="10"/>
+      <c r="A91" s="8"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
       <c r="D91" s="3"/>
@@ -1486,22 +1495,22 @@
       <c r="D94" s="3"/>
     </row>
     <row r="95" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A95" s="8"/>
+      <c r="A95" s="10"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
       <c r="D95" s="3"/>
     </row>
     <row r="96" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A96" s="9"/>
-      <c r="B96" s="5"/>
-      <c r="C96" s="5"/>
-      <c r="D96" s="6"/>
+      <c r="A96" s="8"/>
+      <c r="B96" s="2"/>
+      <c r="C96" s="2"/>
+      <c r="D96" s="3"/>
     </row>
     <row r="97" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A97" s="8"/>
-      <c r="B97" s="2"/>
-      <c r="C97" s="2"/>
-      <c r="D97" s="3"/>
+      <c r="A97" s="9"/>
+      <c r="B97" s="5"/>
+      <c r="C97" s="5"/>
+      <c r="D97" s="6"/>
     </row>
     <row r="98" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="8"/>
@@ -1540,16 +1549,16 @@
       <c r="D103" s="3"/>
     </row>
     <row r="104" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A104" s="9"/>
-      <c r="B104" s="5"/>
-      <c r="C104" s="5"/>
-      <c r="D104" s="6"/>
+      <c r="A104" s="8"/>
+      <c r="B104" s="2"/>
+      <c r="C104" s="2"/>
+      <c r="D104" s="3"/>
     </row>
     <row r="105" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A105" s="8"/>
-      <c r="B105" s="2"/>
-      <c r="C105" s="2"/>
-      <c r="D105" s="3"/>
+      <c r="A105" s="9"/>
+      <c r="B105" s="5"/>
+      <c r="C105" s="5"/>
+      <c r="D105" s="6"/>
     </row>
     <row r="106" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" s="8"/>
@@ -1564,13 +1573,13 @@
       <c r="D107" s="3"/>
     </row>
     <row r="108" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A108" s="10"/>
+      <c r="A108" s="8"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
       <c r="D108" s="3"/>
     </row>
     <row r="109" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A109" s="8"/>
+      <c r="A109" s="10"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
       <c r="D109" s="3"/>
@@ -1594,16 +1603,16 @@
       <c r="D112" s="3"/>
     </row>
     <row r="113" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A113" s="9"/>
-      <c r="B113" s="5"/>
-      <c r="C113" s="5"/>
-      <c r="D113" s="6"/>
+      <c r="A113" s="8"/>
+      <c r="B113" s="2"/>
+      <c r="C113" s="2"/>
+      <c r="D113" s="3"/>
     </row>
     <row r="114" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A114" s="8"/>
-      <c r="B114" s="2"/>
-      <c r="C114" s="2"/>
-      <c r="D114" s="3"/>
+      <c r="A114" s="9"/>
+      <c r="B114" s="5"/>
+      <c r="C114" s="5"/>
+      <c r="D114" s="6"/>
     </row>
     <row r="115" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A115" s="8"/>
@@ -1666,16 +1675,16 @@
       <c r="D124" s="3"/>
     </row>
     <row r="125" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A125" s="9"/>
-      <c r="B125" s="5"/>
-      <c r="C125" s="5"/>
-      <c r="D125" s="6"/>
+      <c r="A125" s="8"/>
+      <c r="B125" s="2"/>
+      <c r="C125" s="2"/>
+      <c r="D125" s="3"/>
     </row>
     <row r="126" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A126" s="8"/>
-      <c r="B126" s="2"/>
-      <c r="C126" s="2"/>
-      <c r="D126" s="3"/>
+      <c r="A126" s="9"/>
+      <c r="B126" s="5"/>
+      <c r="C126" s="5"/>
+      <c r="D126" s="6"/>
     </row>
     <row r="127" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A127" s="8"/>
@@ -1726,16 +1735,16 @@
       <c r="D134" s="3"/>
     </row>
     <row r="135" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A135" s="9"/>
-      <c r="B135" s="5"/>
-      <c r="C135" s="5"/>
-      <c r="D135" s="6"/>
+      <c r="A135" s="8"/>
+      <c r="B135" s="2"/>
+      <c r="C135" s="2"/>
+      <c r="D135" s="3"/>
     </row>
     <row r="136" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A136" s="8"/>
-      <c r="B136" s="2"/>
-      <c r="C136" s="2"/>
-      <c r="D136" s="3"/>
+      <c r="A136" s="9"/>
+      <c r="B136" s="5"/>
+      <c r="C136" s="5"/>
+      <c r="D136" s="6"/>
     </row>
     <row r="137" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A137" s="8"/>
@@ -1810,27 +1819,27 @@
       <c r="D148" s="3"/>
     </row>
     <row r="149" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A149" s="7"/>
-      <c r="B149" s="4"/>
-      <c r="C149" s="4"/>
+      <c r="A149" s="8"/>
+      <c r="B149" s="2"/>
+      <c r="C149" s="2"/>
       <c r="D149" s="3"/>
-      <c r="E149" s="4"/>
-      <c r="F149" s="3"/>
     </row>
     <row r="150" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A150" s="4"/>
-      <c r="B150" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C150" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="A150" s="7"/>
+      <c r="B150" s="4"/>
+      <c r="C150" s="4"/>
       <c r="D150" s="3"/>
+      <c r="E150" s="4"/>
+      <c r="F150" s="3"/>
     </row>
     <row r="151" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A151" s="4"/>
-      <c r="B151" s="4"/>
-      <c r="C151" s="4"/>
+      <c r="B151" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C151" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D151" s="3"/>
     </row>
     <row r="152" spans="1:6" ht="15" x14ac:dyDescent="0.25">
@@ -2017,6 +2026,7 @@
       <c r="A182" s="4"/>
       <c r="B182" s="4"/>
       <c r="C182" s="4"/>
+      <c r="D182" s="3"/>
     </row>
     <row r="183" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A183" s="4"/>
@@ -2024,6 +2034,7 @@
       <c r="C183" s="4"/>
     </row>
     <row r="184" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A184" s="4"/>
       <c r="B184" s="4"/>
       <c r="C184" s="4"/>
     </row>
@@ -2570,6 +2581,10 @@
     <row r="320" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B320" s="4"/>
       <c r="C320" s="4"/>
+    </row>
+    <row r="321" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B321" s="4"/>
+      <c r="C321" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
rally bike v4 - up to last race, 26 frames faster
</commit_message>
<xml_diff>
--- a/RallyBike/FrameCompare.xlsx
+++ b/RallyBike/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\RallyBike\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FE53DC-9FC9-4BFE-9DC2-C75A3332DCE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1524E4-C9A0-47CD-A6D9-823D6CCC973F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45705" yWindow="1350" windowWidth="14490" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="29">
   <si>
     <t>Place</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>Turbo 180</t>
+  </si>
+  <si>
+    <t>Cross bridge</t>
   </si>
 </sst>
 </file>
@@ -602,11 +605,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{315779BE-0457-4CD0-8DEA-0D00DE0D8921}">
-  <dimension ref="A1:F321"/>
+  <dimension ref="A1:F322"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -641,7 +644,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="3">
-        <f t="shared" ref="D2:D38" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
+        <f t="shared" ref="D2:D39" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
         <v>0</v>
       </c>
       <c r="F2" s="2"/>
@@ -970,26 +973,30 @@
       <c r="A25" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="2"/>
+      <c r="B25" s="2">
+        <v>18191</v>
+      </c>
       <c r="C25" s="2">
         <v>18209</v>
       </c>
-      <c r="D25" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D25" s="3">
+        <f t="shared" si="0"/>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="5"/>
+      <c r="B26" s="5">
+        <v>18208</v>
+      </c>
       <c r="C26" s="5">
         <v>18226</v>
       </c>
-      <c r="D26" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D26" s="6">
+        <f t="shared" si="0"/>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1009,175 +1016,202 @@
       <c r="A28" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="2"/>
+      <c r="B28" s="2">
+        <v>18659</v>
+      </c>
       <c r="C28" s="2">
         <v>18677</v>
       </c>
-      <c r="D28" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D28" s="3">
+        <f t="shared" si="0"/>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="5"/>
+      <c r="B29" s="5">
+        <v>18864</v>
+      </c>
       <c r="C29" s="5">
         <v>18882</v>
       </c>
-      <c r="D29" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D29" s="6">
+        <f t="shared" si="0"/>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="2"/>
+      <c r="B30" s="2">
+        <v>18951</v>
+      </c>
       <c r="C30" s="2">
         <v>18969</v>
       </c>
-      <c r="D30" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D30" s="3">
+        <f t="shared" si="0"/>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B31" s="2"/>
+      <c r="A31" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="2">
+        <v>21888</v>
+      </c>
       <c r="C31" s="2">
-        <v>24407</v>
-      </c>
-      <c r="D31" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>21912</v>
+      </c>
+      <c r="D31" s="3">
+        <f t="shared" si="0"/>
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B32" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="B32" s="2">
+        <v>24381</v>
+      </c>
       <c r="C32" s="2">
-        <v>24658</v>
-      </c>
-      <c r="D32" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>24407</v>
+      </c>
+      <c r="D32" s="3">
+        <f t="shared" si="0"/>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B33" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="B33" s="2">
+        <v>24632</v>
+      </c>
       <c r="C33" s="2">
-        <v>24905</v>
-      </c>
-      <c r="D33" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>24658</v>
+      </c>
+      <c r="D33" s="3">
+        <f t="shared" si="0"/>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="2">
+        <v>24879</v>
+      </c>
+      <c r="C34" s="2">
+        <v>24905</v>
+      </c>
+      <c r="D34" s="3">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2">
+      <c r="B35" s="2">
+        <v>24959</v>
+      </c>
+      <c r="C35" s="2">
         <v>24985</v>
       </c>
-      <c r="D34" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="12" t="s">
+      <c r="D35" s="3">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5">
+      <c r="B36" s="5">
+        <v>24980</v>
+      </c>
+      <c r="C36" s="5">
         <v>25006</v>
       </c>
-      <c r="D35" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2">
-        <v>25088</v>
-      </c>
-      <c r="D36" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D36" s="6">
+        <f t="shared" si="0"/>
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B37" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="B37" s="2">
+        <v>25062</v>
+      </c>
       <c r="C37" s="2">
-        <v>29684</v>
-      </c>
-      <c r="D37" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>25088</v>
+      </c>
+      <c r="D37" s="3">
+        <f t="shared" si="0"/>
+        <v>26</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2">
+        <v>29684</v>
+      </c>
+      <c r="D38" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2">
         <v>27669</v>
       </c>
-      <c r="D38" s="3" t="str">
+      <c r="D39" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E39" s="2">
         <v>29677</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F39" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
-      <c r="B39" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="C39" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="D39" s="3"/>
     </row>
     <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
+      <c r="B40" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>2</v>
+      </c>
       <c r="D40" s="3"/>
     </row>
     <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="10"/>
+      <c r="A41" s="8"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="3"/>
     </row>
     <row r="42" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="8"/>
+      <c r="A42" s="10"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="3"/>
@@ -1231,16 +1265,16 @@
       <c r="D50" s="3"/>
     </row>
     <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="9"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="6"/>
+      <c r="A51" s="8"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="3"/>
     </row>
     <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A52" s="8"/>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="3"/>
+      <c r="A52" s="9"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="6"/>
     </row>
     <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="8"/>
@@ -1255,16 +1289,16 @@
       <c r="D54" s="3"/>
     </row>
     <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A55" s="9"/>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="6"/>
+      <c r="A55" s="8"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="3"/>
     </row>
     <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A56" s="8"/>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="3"/>
+      <c r="A56" s="9"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="6"/>
     </row>
     <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="8"/>
@@ -1279,16 +1313,16 @@
       <c r="D58" s="3"/>
     </row>
     <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A59" s="9"/>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="6"/>
+      <c r="A59" s="8"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="3"/>
     </row>
     <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A60" s="8"/>
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
-      <c r="D60" s="3"/>
+      <c r="A60" s="9"/>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="6"/>
     </row>
     <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="8"/>
@@ -1327,16 +1361,16 @@
       <c r="D66" s="3"/>
     </row>
     <row r="67" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A67" s="9"/>
-      <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="6"/>
+      <c r="A67" s="8"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="3"/>
     </row>
     <row r="68" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A68" s="8"/>
-      <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
-      <c r="D68" s="3"/>
+      <c r="A68" s="9"/>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="6"/>
     </row>
     <row r="69" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="8"/>
@@ -1375,16 +1409,16 @@
       <c r="D74" s="3"/>
     </row>
     <row r="75" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A75" s="9"/>
-      <c r="B75" s="5"/>
-      <c r="C75" s="5"/>
-      <c r="D75" s="6"/>
+      <c r="A75" s="8"/>
+      <c r="B75" s="2"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="3"/>
     </row>
     <row r="76" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A76" s="8"/>
-      <c r="B76" s="2"/>
-      <c r="C76" s="2"/>
-      <c r="D76" s="3"/>
+      <c r="A76" s="9"/>
+      <c r="B76" s="5"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="6"/>
     </row>
     <row r="77" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="8"/>
@@ -1423,21 +1457,21 @@
       <c r="D82" s="3"/>
     </row>
     <row r="83" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A83" s="9"/>
-      <c r="B83" s="5"/>
-      <c r="C83" s="5"/>
-      <c r="D83" s="6"/>
+      <c r="A83" s="8"/>
+      <c r="B83" s="2"/>
+      <c r="C83" s="2"/>
+      <c r="D83" s="3"/>
     </row>
     <row r="84" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A84" s="8"/>
-      <c r="B84" s="10"/>
-      <c r="C84" s="10"/>
-      <c r="D84" s="3"/>
+      <c r="A84" s="9"/>
+      <c r="B84" s="5"/>
+      <c r="C84" s="5"/>
+      <c r="D84" s="6"/>
     </row>
     <row r="85" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="8"/>
-      <c r="B85" s="2"/>
-      <c r="C85" s="2"/>
+      <c r="B85" s="10"/>
+      <c r="C85" s="10"/>
       <c r="D85" s="3"/>
     </row>
     <row r="86" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -1465,19 +1499,19 @@
       <c r="D89" s="3"/>
     </row>
     <row r="90" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A90" s="9"/>
-      <c r="B90" s="5"/>
-      <c r="C90" s="5"/>
-      <c r="D90" s="6"/>
+      <c r="A90" s="8"/>
+      <c r="B90" s="2"/>
+      <c r="C90" s="2"/>
+      <c r="D90" s="3"/>
     </row>
     <row r="91" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A91" s="8"/>
-      <c r="B91" s="2"/>
-      <c r="C91" s="2"/>
-      <c r="D91" s="3"/>
+      <c r="A91" s="9"/>
+      <c r="B91" s="5"/>
+      <c r="C91" s="5"/>
+      <c r="D91" s="6"/>
     </row>
     <row r="92" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A92" s="10"/>
+      <c r="A92" s="8"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
       <c r="D92" s="3"/>
@@ -1501,22 +1535,22 @@
       <c r="D95" s="3"/>
     </row>
     <row r="96" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A96" s="8"/>
+      <c r="A96" s="10"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
       <c r="D96" s="3"/>
     </row>
     <row r="97" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A97" s="9"/>
-      <c r="B97" s="5"/>
-      <c r="C97" s="5"/>
-      <c r="D97" s="6"/>
+      <c r="A97" s="8"/>
+      <c r="B97" s="2"/>
+      <c r="C97" s="2"/>
+      <c r="D97" s="3"/>
     </row>
     <row r="98" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A98" s="8"/>
-      <c r="B98" s="2"/>
-      <c r="C98" s="2"/>
-      <c r="D98" s="3"/>
+      <c r="A98" s="9"/>
+      <c r="B98" s="5"/>
+      <c r="C98" s="5"/>
+      <c r="D98" s="6"/>
     </row>
     <row r="99" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="8"/>
@@ -1555,16 +1589,16 @@
       <c r="D104" s="3"/>
     </row>
     <row r="105" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A105" s="9"/>
-      <c r="B105" s="5"/>
-      <c r="C105" s="5"/>
-      <c r="D105" s="6"/>
+      <c r="A105" s="8"/>
+      <c r="B105" s="2"/>
+      <c r="C105" s="2"/>
+      <c r="D105" s="3"/>
     </row>
     <row r="106" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A106" s="8"/>
-      <c r="B106" s="2"/>
-      <c r="C106" s="2"/>
-      <c r="D106" s="3"/>
+      <c r="A106" s="9"/>
+      <c r="B106" s="5"/>
+      <c r="C106" s="5"/>
+      <c r="D106" s="6"/>
     </row>
     <row r="107" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A107" s="8"/>
@@ -1579,13 +1613,13 @@
       <c r="D108" s="3"/>
     </row>
     <row r="109" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A109" s="10"/>
+      <c r="A109" s="8"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
       <c r="D109" s="3"/>
     </row>
     <row r="110" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A110" s="8"/>
+      <c r="A110" s="10"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
       <c r="D110" s="3"/>
@@ -1609,16 +1643,16 @@
       <c r="D113" s="3"/>
     </row>
     <row r="114" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A114" s="9"/>
-      <c r="B114" s="5"/>
-      <c r="C114" s="5"/>
-      <c r="D114" s="6"/>
+      <c r="A114" s="8"/>
+      <c r="B114" s="2"/>
+      <c r="C114" s="2"/>
+      <c r="D114" s="3"/>
     </row>
     <row r="115" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A115" s="8"/>
-      <c r="B115" s="2"/>
-      <c r="C115" s="2"/>
-      <c r="D115" s="3"/>
+      <c r="A115" s="9"/>
+      <c r="B115" s="5"/>
+      <c r="C115" s="5"/>
+      <c r="D115" s="6"/>
     </row>
     <row r="116" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A116" s="8"/>
@@ -1681,16 +1715,16 @@
       <c r="D125" s="3"/>
     </row>
     <row r="126" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A126" s="9"/>
-      <c r="B126" s="5"/>
-      <c r="C126" s="5"/>
-      <c r="D126" s="6"/>
+      <c r="A126" s="8"/>
+      <c r="B126" s="2"/>
+      <c r="C126" s="2"/>
+      <c r="D126" s="3"/>
     </row>
     <row r="127" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A127" s="8"/>
-      <c r="B127" s="2"/>
-      <c r="C127" s="2"/>
-      <c r="D127" s="3"/>
+      <c r="A127" s="9"/>
+      <c r="B127" s="5"/>
+      <c r="C127" s="5"/>
+      <c r="D127" s="6"/>
     </row>
     <row r="128" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A128" s="8"/>
@@ -1741,16 +1775,16 @@
       <c r="D135" s="3"/>
     </row>
     <row r="136" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A136" s="9"/>
-      <c r="B136" s="5"/>
-      <c r="C136" s="5"/>
-      <c r="D136" s="6"/>
+      <c r="A136" s="8"/>
+      <c r="B136" s="2"/>
+      <c r="C136" s="2"/>
+      <c r="D136" s="3"/>
     </row>
     <row r="137" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A137" s="8"/>
-      <c r="B137" s="2"/>
-      <c r="C137" s="2"/>
-      <c r="D137" s="3"/>
+      <c r="A137" s="9"/>
+      <c r="B137" s="5"/>
+      <c r="C137" s="5"/>
+      <c r="D137" s="6"/>
     </row>
     <row r="138" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A138" s="8"/>
@@ -1825,27 +1859,27 @@
       <c r="D149" s="3"/>
     </row>
     <row r="150" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A150" s="7"/>
-      <c r="B150" s="4"/>
-      <c r="C150" s="4"/>
+      <c r="A150" s="8"/>
+      <c r="B150" s="2"/>
+      <c r="C150" s="2"/>
       <c r="D150" s="3"/>
-      <c r="E150" s="4"/>
-      <c r="F150" s="3"/>
     </row>
     <row r="151" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A151" s="4"/>
-      <c r="B151" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C151" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="A151" s="7"/>
+      <c r="B151" s="4"/>
+      <c r="C151" s="4"/>
       <c r="D151" s="3"/>
+      <c r="E151" s="4"/>
+      <c r="F151" s="3"/>
     </row>
     <row r="152" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A152" s="4"/>
-      <c r="B152" s="4"/>
-      <c r="C152" s="4"/>
+      <c r="B152" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C152" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D152" s="3"/>
     </row>
     <row r="153" spans="1:6" ht="15" x14ac:dyDescent="0.25">
@@ -2032,6 +2066,7 @@
       <c r="A183" s="4"/>
       <c r="B183" s="4"/>
       <c r="C183" s="4"/>
+      <c r="D183" s="3"/>
     </row>
     <row r="184" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A184" s="4"/>
@@ -2039,6 +2074,7 @@
       <c r="C184" s="4"/>
     </row>
     <row r="185" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A185" s="4"/>
       <c r="B185" s="4"/>
       <c r="C185" s="4"/>
     </row>
@@ -2585,6 +2621,10 @@
     <row r="321" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B321" s="4"/>
       <c r="C321" s="4"/>
+    </row>
+    <row r="322" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B322" s="4"/>
+      <c r="C322" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
rally bike v4 - up to the point that needs an invuln manip
</commit_message>
<xml_diff>
--- a/RallyBike/FrameCompare.xlsx
+++ b/RallyBike/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\RallyBike\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1524E4-C9A0-47CD-A6D9-823D6CCC973F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F166FA8D-6234-4F25-A2CD-615F77FE853D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45705" yWindow="1350" windowWidth="14490" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="31">
   <si>
     <t>Place</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>Cross bridge</t>
+  </si>
+  <si>
+    <t>get turbo</t>
+  </si>
+  <si>
+    <t>40th place</t>
   </si>
 </sst>
 </file>
@@ -605,11 +611,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{315779BE-0457-4CD0-8DEA-0D00DE0D8921}">
-  <dimension ref="A1:F322"/>
+  <dimension ref="A1:F323"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B38" sqref="B38"/>
+      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -644,7 +650,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="3">
-        <f t="shared" ref="D2:D39" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
+        <f t="shared" ref="D2:D40" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
         <v>0</v>
       </c>
       <c r="F2" s="2"/>
@@ -1163,21 +1169,26 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B38" s="2"/>
+      <c r="A38" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38" s="2">
+        <v>26368</v>
+      </c>
       <c r="C38" s="2">
-        <v>29684</v>
-      </c>
-      <c r="D38" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>26394</v>
+      </c>
+      <c r="D38" s="3">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="E38" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2">
@@ -1187,37 +1198,44 @@
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E39" s="2">
+    </row>
+    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2">
+        <v>27669</v>
+      </c>
+      <c r="D40" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="E40" s="2">
         <v>29677</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F40" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="8"/>
-      <c r="B40" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="C40" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="D40" s="3"/>
     </row>
     <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
+      <c r="B41" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>2</v>
+      </c>
       <c r="D41" s="3"/>
     </row>
     <row r="42" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="10"/>
+      <c r="A42" s="8"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="3"/>
     </row>
     <row r="43" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="8"/>
+      <c r="A43" s="10"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="3"/>
@@ -1271,16 +1289,16 @@
       <c r="D51" s="3"/>
     </row>
     <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A52" s="9"/>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="6"/>
+      <c r="A52" s="8"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="3"/>
     </row>
     <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="8"/>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="3"/>
+      <c r="A53" s="9"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="6"/>
     </row>
     <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="8"/>
@@ -1295,16 +1313,16 @@
       <c r="D55" s="3"/>
     </row>
     <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A56" s="9"/>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="6"/>
+      <c r="A56" s="8"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="3"/>
     </row>
     <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A57" s="8"/>
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="3"/>
+      <c r="A57" s="9"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="6"/>
     </row>
     <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="8"/>
@@ -1319,16 +1337,16 @@
       <c r="D59" s="3"/>
     </row>
     <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A60" s="9"/>
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="6"/>
+      <c r="A60" s="8"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="3"/>
     </row>
     <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A61" s="8"/>
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="3"/>
+      <c r="A61" s="9"/>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="6"/>
     </row>
     <row r="62" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="8"/>
@@ -1367,16 +1385,16 @@
       <c r="D67" s="3"/>
     </row>
     <row r="68" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A68" s="9"/>
-      <c r="B68" s="5"/>
-      <c r="C68" s="5"/>
-      <c r="D68" s="6"/>
+      <c r="A68" s="8"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="3"/>
     </row>
     <row r="69" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A69" s="8"/>
-      <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
-      <c r="D69" s="3"/>
+      <c r="A69" s="9"/>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="6"/>
     </row>
     <row r="70" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="8"/>
@@ -1415,16 +1433,16 @@
       <c r="D75" s="3"/>
     </row>
     <row r="76" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A76" s="9"/>
-      <c r="B76" s="5"/>
-      <c r="C76" s="5"/>
-      <c r="D76" s="6"/>
+      <c r="A76" s="8"/>
+      <c r="B76" s="2"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="3"/>
     </row>
     <row r="77" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A77" s="8"/>
-      <c r="B77" s="2"/>
-      <c r="C77" s="2"/>
-      <c r="D77" s="3"/>
+      <c r="A77" s="9"/>
+      <c r="B77" s="5"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="6"/>
     </row>
     <row r="78" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="8"/>
@@ -1463,21 +1481,21 @@
       <c r="D83" s="3"/>
     </row>
     <row r="84" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A84" s="9"/>
-      <c r="B84" s="5"/>
-      <c r="C84" s="5"/>
-      <c r="D84" s="6"/>
+      <c r="A84" s="8"/>
+      <c r="B84" s="2"/>
+      <c r="C84" s="2"/>
+      <c r="D84" s="3"/>
     </row>
     <row r="85" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A85" s="8"/>
-      <c r="B85" s="10"/>
-      <c r="C85" s="10"/>
-      <c r="D85" s="3"/>
+      <c r="A85" s="9"/>
+      <c r="B85" s="5"/>
+      <c r="C85" s="5"/>
+      <c r="D85" s="6"/>
     </row>
     <row r="86" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="8"/>
-      <c r="B86" s="2"/>
-      <c r="C86" s="2"/>
+      <c r="B86" s="10"/>
+      <c r="C86" s="10"/>
       <c r="D86" s="3"/>
     </row>
     <row r="87" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -1505,19 +1523,19 @@
       <c r="D90" s="3"/>
     </row>
     <row r="91" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A91" s="9"/>
-      <c r="B91" s="5"/>
-      <c r="C91" s="5"/>
-      <c r="D91" s="6"/>
+      <c r="A91" s="8"/>
+      <c r="B91" s="2"/>
+      <c r="C91" s="2"/>
+      <c r="D91" s="3"/>
     </row>
     <row r="92" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A92" s="8"/>
-      <c r="B92" s="2"/>
-      <c r="C92" s="2"/>
-      <c r="D92" s="3"/>
+      <c r="A92" s="9"/>
+      <c r="B92" s="5"/>
+      <c r="C92" s="5"/>
+      <c r="D92" s="6"/>
     </row>
     <row r="93" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A93" s="10"/>
+      <c r="A93" s="8"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
       <c r="D93" s="3"/>
@@ -1541,22 +1559,22 @@
       <c r="D96" s="3"/>
     </row>
     <row r="97" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A97" s="8"/>
+      <c r="A97" s="10"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
       <c r="D97" s="3"/>
     </row>
     <row r="98" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A98" s="9"/>
-      <c r="B98" s="5"/>
-      <c r="C98" s="5"/>
-      <c r="D98" s="6"/>
+      <c r="A98" s="8"/>
+      <c r="B98" s="2"/>
+      <c r="C98" s="2"/>
+      <c r="D98" s="3"/>
     </row>
     <row r="99" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A99" s="8"/>
-      <c r="B99" s="2"/>
-      <c r="C99" s="2"/>
-      <c r="D99" s="3"/>
+      <c r="A99" s="9"/>
+      <c r="B99" s="5"/>
+      <c r="C99" s="5"/>
+      <c r="D99" s="6"/>
     </row>
     <row r="100" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="8"/>
@@ -1595,16 +1613,16 @@
       <c r="D105" s="3"/>
     </row>
     <row r="106" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A106" s="9"/>
-      <c r="B106" s="5"/>
-      <c r="C106" s="5"/>
-      <c r="D106" s="6"/>
+      <c r="A106" s="8"/>
+      <c r="B106" s="2"/>
+      <c r="C106" s="2"/>
+      <c r="D106" s="3"/>
     </row>
     <row r="107" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A107" s="8"/>
-      <c r="B107" s="2"/>
-      <c r="C107" s="2"/>
-      <c r="D107" s="3"/>
+      <c r="A107" s="9"/>
+      <c r="B107" s="5"/>
+      <c r="C107" s="5"/>
+      <c r="D107" s="6"/>
     </row>
     <row r="108" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A108" s="8"/>
@@ -1619,13 +1637,13 @@
       <c r="D109" s="3"/>
     </row>
     <row r="110" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A110" s="10"/>
+      <c r="A110" s="8"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
       <c r="D110" s="3"/>
     </row>
     <row r="111" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A111" s="8"/>
+      <c r="A111" s="10"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
       <c r="D111" s="3"/>
@@ -1649,16 +1667,16 @@
       <c r="D114" s="3"/>
     </row>
     <row r="115" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A115" s="9"/>
-      <c r="B115" s="5"/>
-      <c r="C115" s="5"/>
-      <c r="D115" s="6"/>
+      <c r="A115" s="8"/>
+      <c r="B115" s="2"/>
+      <c r="C115" s="2"/>
+      <c r="D115" s="3"/>
     </row>
     <row r="116" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A116" s="8"/>
-      <c r="B116" s="2"/>
-      <c r="C116" s="2"/>
-      <c r="D116" s="3"/>
+      <c r="A116" s="9"/>
+      <c r="B116" s="5"/>
+      <c r="C116" s="5"/>
+      <c r="D116" s="6"/>
     </row>
     <row r="117" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A117" s="8"/>
@@ -1721,16 +1739,16 @@
       <c r="D126" s="3"/>
     </row>
     <row r="127" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A127" s="9"/>
-      <c r="B127" s="5"/>
-      <c r="C127" s="5"/>
-      <c r="D127" s="6"/>
+      <c r="A127" s="8"/>
+      <c r="B127" s="2"/>
+      <c r="C127" s="2"/>
+      <c r="D127" s="3"/>
     </row>
     <row r="128" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A128" s="8"/>
-      <c r="B128" s="2"/>
-      <c r="C128" s="2"/>
-      <c r="D128" s="3"/>
+      <c r="A128" s="9"/>
+      <c r="B128" s="5"/>
+      <c r="C128" s="5"/>
+      <c r="D128" s="6"/>
     </row>
     <row r="129" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A129" s="8"/>
@@ -1781,16 +1799,16 @@
       <c r="D136" s="3"/>
     </row>
     <row r="137" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A137" s="9"/>
-      <c r="B137" s="5"/>
-      <c r="C137" s="5"/>
-      <c r="D137" s="6"/>
+      <c r="A137" s="8"/>
+      <c r="B137" s="2"/>
+      <c r="C137" s="2"/>
+      <c r="D137" s="3"/>
     </row>
     <row r="138" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A138" s="8"/>
-      <c r="B138" s="2"/>
-      <c r="C138" s="2"/>
-      <c r="D138" s="3"/>
+      <c r="A138" s="9"/>
+      <c r="B138" s="5"/>
+      <c r="C138" s="5"/>
+      <c r="D138" s="6"/>
     </row>
     <row r="139" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A139" s="8"/>
@@ -1865,27 +1883,27 @@
       <c r="D150" s="3"/>
     </row>
     <row r="151" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A151" s="7"/>
-      <c r="B151" s="4"/>
-      <c r="C151" s="4"/>
+      <c r="A151" s="8"/>
+      <c r="B151" s="2"/>
+      <c r="C151" s="2"/>
       <c r="D151" s="3"/>
-      <c r="E151" s="4"/>
-      <c r="F151" s="3"/>
     </row>
     <row r="152" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A152" s="4"/>
-      <c r="B152" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C152" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="A152" s="7"/>
+      <c r="B152" s="4"/>
+      <c r="C152" s="4"/>
       <c r="D152" s="3"/>
+      <c r="E152" s="4"/>
+      <c r="F152" s="3"/>
     </row>
     <row r="153" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A153" s="4"/>
-      <c r="B153" s="4"/>
-      <c r="C153" s="4"/>
+      <c r="B153" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C153" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D153" s="3"/>
     </row>
     <row r="154" spans="1:6" ht="15" x14ac:dyDescent="0.25">
@@ -2072,6 +2090,7 @@
       <c r="A184" s="4"/>
       <c r="B184" s="4"/>
       <c r="C184" s="4"/>
+      <c r="D184" s="3"/>
     </row>
     <row r="185" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A185" s="4"/>
@@ -2079,6 +2098,7 @@
       <c r="C185" s="4"/>
     </row>
     <row r="186" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A186" s="4"/>
       <c r="B186" s="4"/>
       <c r="C186" s="4"/>
     </row>
@@ -2625,6 +2645,10 @@
     <row r="322" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B322" s="4"/>
       <c r="C322" s="4"/>
+    </row>
+    <row r="323" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B323" s="4"/>
+      <c r="C323" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
v4 with earlier input than v3, with new strat, don't try to get invuln on 2nd heli, 241 frames faster
</commit_message>
<xml_diff>
--- a/RallyBike/FrameCompare.xlsx
+++ b/RallyBike/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\RallyBike\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F166FA8D-6234-4F25-A2CD-615F77FE853D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE7DD51-46F1-4DB3-A82E-47F6CAE3B9AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45705" yWindow="1350" windowWidth="14490" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -615,7 +615,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
+      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1203,13 +1203,15 @@
       <c r="A40" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B40" s="2"/>
+      <c r="B40" s="2">
+        <v>27428</v>
+      </c>
       <c r="C40" s="2">
         <v>27669</v>
       </c>
-      <c r="D40" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D40" s="3">
+        <f t="shared" si="0"/>
+        <v>241</v>
       </c>
       <c r="E40" s="2">
         <v>29677</v>

</xml_diff>

<commit_message>
rally bike v4 - down to 27368
</commit_message>
<xml_diff>
--- a/RallyBike/FrameCompare.xlsx
+++ b/RallyBike/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\RallyBike\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE7DD51-46F1-4DB3-A82E-47F6CAE3B9AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF6BB91C-324D-466C-A06F-3F3A16556FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45705" yWindow="1350" windowWidth="14490" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1204,14 +1204,14 @@
         <v>20</v>
       </c>
       <c r="B40" s="2">
-        <v>27428</v>
+        <v>27368</v>
       </c>
       <c r="C40" s="2">
         <v>27669</v>
       </c>
       <c r="D40" s="3">
         <f t="shared" si="0"/>
-        <v>241</v>
+        <v>301</v>
       </c>
       <c r="E40" s="2">
         <v>29677</v>

</xml_diff>

<commit_message>
Rally bike v4 done
</commit_message>
<xml_diff>
--- a/RallyBike/FrameCompare.xlsx
+++ b/RallyBike/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\RallyBike\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C54469-549E-4CAC-958E-C8F26E9E6052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E911FCE-E384-4A7B-8969-3ABA7C88DED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1204,14 +1204,14 @@
         <v>20</v>
       </c>
       <c r="B40" s="2">
-        <v>27248</v>
+        <v>27240</v>
       </c>
       <c r="C40" s="2">
         <v>27669</v>
       </c>
       <c r="D40" s="3">
         <f t="shared" si="0"/>
-        <v>421</v>
+        <v>429</v>
       </c>
       <c r="E40" s="2">
         <v>29677</v>

</xml_diff>